<commit_message>
Refactoring and excel template
</commit_message>
<xml_diff>
--- a/Recon2.0_Template.xlsx
+++ b/Recon2.0_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saiprasadkrishnamurthy/2.0/reconciliation-engine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{536723E4-D4FA-D944-A257-41343EA9B98C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7769604D-863C-E44F-B05D-0082F51AD292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20740" xr2:uid="{C08B0C19-EF01-7B46-898D-9F2EEE986A3C}"/>
   </bookViews>
@@ -575,7 +575,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
scaling with push consumer
</commit_message>
<xml_diff>
--- a/Recon2.0_Template.xlsx
+++ b/Recon2.0_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saiprasadkrishnamurthy/2.0/reconciliation-engine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7769604D-863C-E44F-B05D-0082F51AD292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B36DF3F9-51EE-9B4F-BBAC-DB9D45362ECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20740" xr2:uid="{C08B0C19-EF01-7B46-898D-9F2EEE986A3C}"/>
   </bookViews>
@@ -575,7 +575,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>